<commit_message>
changes in opt-in column
</commit_message>
<xml_diff>
--- a/excel_data/Book24.xlsx
+++ b/excel_data/Book24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TME-1\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBD5C1B-A4F0-4A68-882B-3584F2B214CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66112D7-2364-4161-B8E2-12824D303408}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E479D578-BD8A-4895-B658-716D462F331C}"/>
   </bookViews>
@@ -2911,8 +2911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A7637C-B6C0-45EB-BF4B-9D78094334E4}">
   <dimension ref="A1:Q162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C104" sqref="A104:XFD104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5975,22 +5975,22 @@
         <v>283</v>
       </c>
       <c r="C104" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="D104" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="E104" t="s">
         <v>20</v>
       </c>
       <c r="F104" t="s">
-        <v>334</v>
+        <v>280</v>
       </c>
       <c r="H104" t="s">
         <v>20</v>
       </c>
       <c r="I104" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="K104" s="2"/>
       <c r="L104" t="s">
@@ -6003,7 +6003,7 @@
         <v>282</v>
       </c>
       <c r="Q104" t="s">
-        <v>286</v>
+        <v>340</v>
       </c>
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
@@ -6011,10 +6011,10 @@
         <v>283</v>
       </c>
       <c r="C105" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D105" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E105" t="s">
         <v>20</v>
@@ -6026,7 +6026,7 @@
         <v>20</v>
       </c>
       <c r="I105" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="K105" s="2"/>
       <c r="L105" t="s">
@@ -6047,22 +6047,22 @@
         <v>283</v>
       </c>
       <c r="C106" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D106" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E106" t="s">
         <v>20</v>
       </c>
       <c r="F106" t="s">
-        <v>280</v>
+        <v>334</v>
       </c>
       <c r="H106" t="s">
         <v>20</v>
       </c>
       <c r="I106" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="K106" s="2"/>
       <c r="L106" t="s">
@@ -6075,7 +6075,7 @@
         <v>282</v>
       </c>
       <c r="Q106" t="s">
-        <v>340</v>
+        <v>286</v>
       </c>
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
takenstyle backup and created formatted style, applied blue color on hover of multiselect
</commit_message>
<xml_diff>
--- a/excel_data/Book24.xlsx
+++ b/excel_data/Book24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TME-1\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66112D7-2364-4161-B8E2-12824D303408}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EBBBF9-9672-446F-929F-A9C09C0273E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E479D578-BD8A-4895-B658-716D462F331C}"/>
   </bookViews>
@@ -2911,8 +2911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7A7637C-B6C0-45EB-BF4B-9D78094334E4}">
   <dimension ref="A1:Q162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="70" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C104" sqref="A104:XFD104"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>